<commit_message>
test code for generating new arrays
</commit_message>
<xml_diff>
--- a/predicted_trajectories.xlsx
+++ b/predicted_trajectories.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,810 +447,458 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="B2" t="n">
-        <v>834.1172537163824</v>
+        <v>3077.162513269976</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="B3" t="n">
-        <v>834.1172537163824</v>
+        <v>4092.015648792559</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="B4" t="n">
-        <v>2830.770215897365</v>
+        <v>4709.498630076444</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="B5" t="n">
-        <v>2830.770215897365</v>
+        <v>5238.650352021337</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.04</v>
+        <v>0.17</v>
       </c>
       <c r="B6" t="n">
-        <v>3225.364158193556</v>
+        <v>5693.080605876607</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="B7" t="n">
-        <v>3696.836508034739</v>
+        <v>5863.171644560897</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.06</v>
+        <v>0.23</v>
       </c>
       <c r="B8" t="n">
-        <v>3721.361598147059</v>
+        <v>6331.200899832631</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="B9" t="n">
-        <v>4040.892062790728</v>
+        <v>6698.497324937877</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="B10" t="n">
-        <v>4040.892062790728</v>
+        <v>6906.319319641068</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.09</v>
+        <v>0.3300000000000001</v>
       </c>
       <c r="B11" t="n">
-        <v>4343.667486639863</v>
+        <v>7093.349864450093</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.1</v>
+        <v>0.3700000000000001</v>
       </c>
       <c r="B12" t="n">
-        <v>4432.808196265737</v>
+        <v>7331.737722785797</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="B13" t="n">
-        <v>4432.808196265737</v>
+        <v>7398.478288688837</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.12</v>
+        <v>0.43</v>
       </c>
       <c r="B14" t="n">
-        <v>4892.07645167559</v>
+        <v>7669.54504942052</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.13</v>
+        <v>0.47</v>
       </c>
       <c r="B15" t="n">
-        <v>4892.07645167559</v>
+        <v>7857.838097332378</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.14</v>
+        <v>0.5</v>
       </c>
       <c r="B16" t="n">
-        <v>4892.156367617734</v>
+        <v>7962.96903945955</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.15</v>
+        <v>0.53</v>
       </c>
       <c r="B17" t="n">
-        <v>5252.91190553838</v>
+        <v>7898.640174301781</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.16</v>
+        <v>0.5700000000000001</v>
       </c>
       <c r="B18" t="n">
-        <v>5252.91190553838</v>
+        <v>8040.269317703791</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.17</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="B19" t="n">
-        <v>5252.91190553838</v>
+        <v>8083.525844706185</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.18</v>
+        <v>0.6300000000000001</v>
       </c>
       <c r="B20" t="n">
-        <v>5252.91190553838</v>
+        <v>8132.924005701289</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.19</v>
+        <v>0.6700000000000002</v>
       </c>
       <c r="B21" t="n">
-        <v>5481.941162719432</v>
+        <v>8353.570209014373</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.2</v>
+        <v>0.7000000000000002</v>
       </c>
       <c r="B22" t="n">
-        <v>5481.941162719432</v>
+        <v>8368.816707893682</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.21</v>
+        <v>0.7300000000000002</v>
       </c>
       <c r="B23" t="n">
-        <v>5662.367918083667</v>
+        <v>8394.334141484829</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.22</v>
+        <v>0.7700000000000002</v>
       </c>
       <c r="B24" t="n">
-        <v>5719.411973238221</v>
+        <v>8406.355288039766</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.23</v>
+        <v>0.8000000000000003</v>
       </c>
       <c r="B25" t="n">
-        <v>5719.411973238221</v>
+        <v>8422.872370634068</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.24</v>
+        <v>0.8300000000000003</v>
       </c>
       <c r="B26" t="n">
-        <v>5766.794856266129</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.25</v>
+        <v>0.8700000000000003</v>
       </c>
       <c r="B27" t="n">
-        <v>5766.794856266129</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.26</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="B28" t="n">
-        <v>6094.445024828155</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.27</v>
+        <v>0.9300000000000004</v>
       </c>
       <c r="B29" t="n">
-        <v>6099.442217773368</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.28</v>
+        <v>0.9700000000000004</v>
       </c>
       <c r="B30" t="n">
-        <v>6099.442217773368</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.29</v>
+        <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>6300.380814212744</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3</v>
+        <v>1.03</v>
       </c>
       <c r="B32" t="n">
-        <v>6300.380814212744</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.31</v>
+        <v>1.070000000000001</v>
       </c>
       <c r="B33" t="n">
-        <v>6300.381469535163</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.32</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="B34" t="n">
-        <v>6443.575216429293</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.33</v>
+        <v>1.130000000000001</v>
       </c>
       <c r="B35" t="n">
-        <v>6443.575216466676</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.34</v>
+        <v>1.170000000000001</v>
       </c>
       <c r="B36" t="n">
-        <v>6516.639325821726</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.35</v>
+        <v>1.200000000000001</v>
       </c>
       <c r="B37" t="n">
-        <v>6516.639325821726</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.36</v>
+        <v>1.230000000000001</v>
       </c>
       <c r="B38" t="n">
-        <v>6686.149747931003</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.37</v>
+        <v>1.270000000000001</v>
       </c>
       <c r="B39" t="n">
-        <v>6686.704690168023</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.38</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="B40" t="n">
-        <v>6686.704690168023</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.39</v>
+        <v>1.330000000000001</v>
       </c>
       <c r="B41" t="n">
-        <v>6817.930027128903</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.4</v>
+        <v>1.370000000000001</v>
       </c>
       <c r="B42" t="n">
-        <v>6817.930027128903</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.41</v>
+        <v>1.400000000000001</v>
       </c>
       <c r="B43" t="n">
-        <v>6873.174337851673</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.42</v>
+        <v>1.430000000000001</v>
       </c>
       <c r="B44" t="n">
-        <v>7051.251573615705</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.43</v>
+        <v>1.470000000000001</v>
       </c>
       <c r="B45" t="n">
-        <v>7051.251573615705</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.44</v>
+        <v>1.500000000000001</v>
       </c>
       <c r="B46" t="n">
-        <v>7054.505329625024</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.45</v>
+        <v>1.530000000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>7054.505329625024</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.46</v>
+        <v>1.570000000000001</v>
       </c>
       <c r="B48" t="n">
-        <v>7144.156641074791</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.47</v>
+        <v>1.600000000000001</v>
       </c>
       <c r="B49" t="n">
-        <v>7238.611677549092</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.48</v>
+        <v>1.630000000000001</v>
       </c>
       <c r="B50" t="n">
-        <v>7238.611677549092</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.49</v>
+        <v>1.670000000000001</v>
       </c>
       <c r="B51" t="n">
-        <v>7320.726099540881</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.5</v>
+        <v>1.700000000000001</v>
       </c>
       <c r="B52" t="n">
-        <v>7320.726099540881</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.51</v>
+        <v>1.730000000000001</v>
       </c>
       <c r="B53" t="n">
-        <v>7320.726099540881</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.52</v>
+        <v>1.770000000000001</v>
       </c>
       <c r="B54" t="n">
-        <v>7494.125917138773</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.53</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="B55" t="n">
-        <v>7494.125917138773</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.54</v>
+        <v>1.830000000000001</v>
       </c>
       <c r="B56" t="n">
-        <v>7494.125917138773</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.55</v>
+        <v>1.870000000000001</v>
       </c>
       <c r="B57" t="n">
-        <v>7541.201137816073</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.900000000000001</v>
       </c>
       <c r="B58" t="n">
-        <v>7637.968309700131</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>0.5700000000000001</v>
-      </c>
-      <c r="B59" t="n">
-        <v>7666.827038508944</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>7666.827038508944</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>7750.185003211747</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="B62" t="n">
-        <v>7750.185003711744</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>7750.185003711744</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>7804.170892430811</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>7804.170892430811</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>7874.938058189447</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="B67" t="n">
-        <v>7874.938058189447</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>7991.226278192024</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>7991.672650349887</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>0.68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>7991.672650349887</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>0.6900000000000001</v>
-      </c>
-      <c r="B71" t="n">
-        <v>8037.509491430862</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>0.7000000000000001</v>
-      </c>
-      <c r="B72" t="n">
-        <v>8037.509491430862</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>8039.47693680538</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="B74" t="n">
-        <v>8096.320371477505</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>8096.320371477505</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>8096.320371477505</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>8096.320371477505</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>8122.241399231748</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>8122.241399231748</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>8122.241399231748</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>0.79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>8159.719998741552</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="B82" t="n">
-        <v>8159.719998741552</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="B83" t="n">
-        <v>8159.719998741552</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>0.8200000000000001</v>
-      </c>
-      <c r="B84" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>0.8300000000000001</v>
-      </c>
-      <c r="B85" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="B86" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="B87" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="B88" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="B89" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="B90" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="B91" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="B92" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>0.91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>0.9400000000000001</v>
-      </c>
-      <c r="B96" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>0.9500000000000001</v>
-      </c>
-      <c r="B97" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="B98" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="B99" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="B100" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>8165.018598087261</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>1</v>
-      </c>
-      <c r="B102" t="n">
-        <v>8165.018598087261</v>
+        <v>8425.207500664945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>